<commit_message>
Gannt & Scrum nachgeführt
</commit_message>
<xml_diff>
--- a/Restaurants_Vallah_SJ/Documentation/210_Gantt-Diagramm.110_Sebastian_Joel.xlsx
+++ b/Restaurants_Vallah_SJ/Documentation/210_Gantt-Diagramm.110_Sebastian_Joel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
   <si>
     <t>Nr.</t>
   </si>
@@ -85,9 +85,6 @@
     <t>US 03 "Als User möchte ich für jede Küche alle Restaurants angezeigt bekommen."</t>
   </si>
   <si>
-    <t xml:space="preserve">5h / </t>
-  </si>
-  <si>
     <t>8h /</t>
   </si>
   <si>
@@ -116,6 +113,15 @@
   </si>
   <si>
     <t>US 09 "Als Benutzer möchte ich registrieren können."</t>
+  </si>
+  <si>
+    <t>5h / 4h</t>
+  </si>
+  <si>
+    <t>5h / 6h</t>
+  </si>
+  <si>
+    <t>8h / 10h</t>
   </si>
 </sst>
 </file>
@@ -448,106 +454,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -556,15 +463,114 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -880,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AW26" sqref="AW26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +930,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="24"/>
@@ -935,109 +941,109 @@
       <c r="E1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="87">
+      <c r="F1" s="56">
         <v>43129</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="87">
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="56">
         <v>43136</v>
       </c>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="87">
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="56">
         <v>43137</v>
       </c>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="87">
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="56">
         <v>43138</v>
       </c>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="66"/>
-      <c r="AJ1" s="66"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="87">
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="55"/>
+      <c r="AL1" s="56">
         <v>43139</v>
       </c>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="87">
-        <v>43140</v>
-      </c>
-      <c r="AU1" s="66"/>
-      <c r="AV1" s="66"/>
-      <c r="AW1" s="66"/>
-      <c r="AX1" s="66"/>
-      <c r="AY1" s="66"/>
-      <c r="AZ1" s="66"/>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="65" t="s">
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="55"/>
+      <c r="AT1" s="56">
+        <v>43150</v>
+      </c>
+      <c r="AU1" s="54"/>
+      <c r="AV1" s="54"/>
+      <c r="AW1" s="54"/>
+      <c r="AX1" s="54"/>
+      <c r="AY1" s="54"/>
+      <c r="AZ1" s="54"/>
+      <c r="BA1" s="55"/>
+      <c r="BB1" s="56">
+        <v>43151</v>
+      </c>
+      <c r="BC1" s="54"/>
+      <c r="BD1" s="54"/>
+      <c r="BE1" s="54"/>
+      <c r="BF1" s="54"/>
+      <c r="BG1" s="54"/>
+      <c r="BH1" s="54"/>
+      <c r="BI1" s="55"/>
+      <c r="BJ1" s="56">
+        <v>43152</v>
+      </c>
+      <c r="BK1" s="54"/>
+      <c r="BL1" s="54"/>
+      <c r="BM1" s="54"/>
+      <c r="BN1" s="54"/>
+      <c r="BO1" s="54"/>
+      <c r="BP1" s="54"/>
+      <c r="BQ1" s="55"/>
+      <c r="BR1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="BC1" s="66"/>
-      <c r="BD1" s="66"/>
-      <c r="BE1" s="66"/>
-      <c r="BF1" s="66"/>
-      <c r="BG1" s="66"/>
-      <c r="BH1" s="66"/>
-      <c r="BI1" s="67"/>
-      <c r="BJ1" s="65" t="s">
+      <c r="BS1" s="54"/>
+      <c r="BT1" s="54"/>
+      <c r="BU1" s="54"/>
+      <c r="BV1" s="54"/>
+      <c r="BW1" s="54"/>
+      <c r="BX1" s="54"/>
+      <c r="BY1" s="55"/>
+      <c r="BZ1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="BK1" s="66"/>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="66"/>
-      <c r="BN1" s="66"/>
-      <c r="BO1" s="66"/>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="BS1" s="66"/>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="66"/>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="66"/>
-      <c r="CC1" s="66"/>
-      <c r="CD1" s="66"/>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="67"/>
+      <c r="CA1" s="54"/>
+      <c r="CB1" s="54"/>
+      <c r="CC1" s="54"/>
+      <c r="CD1" s="54"/>
+      <c r="CE1" s="54"/>
+      <c r="CF1" s="54"/>
+      <c r="CG1" s="55"/>
     </row>
     <row r="2" spans="1:85" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
+      <c r="A2" s="76"/>
       <c r="B2" s="22" t="s">
         <v>13</v>
       </c>
@@ -1290,23 +1296,23 @@
       </c>
     </row>
     <row r="3" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62">
+      <c r="A3" s="60">
         <v>1</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="68" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D3" s="68"/>
       <c r="E3" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="79"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="81"/>
       <c r="M3" s="11"/>
       <c r="N3" s="9"/>
       <c r="U3" s="11"/>
@@ -1328,8 +1334,8 @@
       <c r="CG3" s="11"/>
     </row>
     <row r="4" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="60"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="78"/>
       <c r="C4" s="69"/>
       <c r="D4" s="69"/>
       <c r="E4" s="40" t="s">
@@ -1347,8 +1353,8 @@
       <c r="CG4" s="13"/>
     </row>
     <row r="5" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="60"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="78"/>
       <c r="C5" s="69"/>
       <c r="D5" s="69"/>
       <c r="E5" s="41" t="s">
@@ -1371,8 +1377,8 @@
       <c r="CG5" s="13"/>
     </row>
     <row r="6" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="61"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="70"/>
       <c r="D6" s="70"/>
       <c r="E6" s="40" t="s">
@@ -1386,10 +1392,10 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="13"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
@@ -1460,22 +1466,22 @@
       <c r="CG6" s="13"/>
     </row>
     <row r="7" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62">
+      <c r="A7" s="60">
         <v>2</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="74"/>
-      <c r="E7" s="80" t="s">
+      <c r="D7" s="72"/>
+      <c r="E7" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="84"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
       <c r="M7" s="17"/>
       <c r="N7" s="15"/>
       <c r="U7" s="17"/>
@@ -1497,14 +1503,14 @@
       <c r="CG7" s="17"/>
     </row>
     <row r="8" spans="1:85" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="81" t="s">
+      <c r="A8" s="60"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="86"/>
+      <c r="F8" s="52"/>
       <c r="G8" s="23"/>
       <c r="M8" s="20"/>
       <c r="U8" s="20"/>
@@ -1525,14 +1531,14 @@
       <c r="CG8" s="20"/>
     </row>
     <row r="9" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="82" t="s">
+      <c r="A9" s="60"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="85"/>
+      <c r="F9" s="51"/>
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
       <c r="M9" s="20"/>
@@ -1554,14 +1560,14 @@
       <c r="CG9" s="20"/>
     </row>
     <row r="10" spans="1:85" s="21" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="81" t="s">
+      <c r="A10" s="60"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="86"/>
+      <c r="F10" s="52"/>
       <c r="G10" s="23"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
@@ -1643,14 +1649,14 @@
       <c r="CG10" s="20"/>
     </row>
     <row r="11" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62">
+      <c r="A11" s="60">
         <v>3</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="57" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="68" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D11" s="68"/>
       <c r="E11" s="39" t="s">
@@ -1678,8 +1684,8 @@
       <c r="CG11" s="11"/>
     </row>
     <row r="12" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="69"/>
       <c r="D12" s="69"/>
       <c r="E12" s="40" t="s">
@@ -1697,8 +1703,8 @@
       <c r="CG12" s="13"/>
     </row>
     <row r="13" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
-      <c r="B13" s="47"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="69"/>
       <c r="D13" s="69"/>
       <c r="E13" s="41" t="s">
@@ -1724,8 +1730,8 @@
       <c r="CG13" s="13"/>
     </row>
     <row r="14" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="B14" s="48"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="70"/>
       <c r="D14" s="70"/>
       <c r="E14" s="40" t="s">
@@ -1747,19 +1753,19 @@
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="13"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
       <c r="AC14" s="13"/>
-      <c r="AD14" s="12"/>
-      <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
-      <c r="AG14" s="12"/>
-      <c r="AH14" s="12"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="23"/>
+      <c r="AF14" s="23"/>
+      <c r="AG14" s="23"/>
+      <c r="AH14" s="23"/>
       <c r="AI14" s="12"/>
       <c r="AJ14" s="12"/>
       <c r="AK14" s="13"/>
@@ -1813,28 +1819,28 @@
       <c r="CG14" s="13"/>
     </row>
     <row r="15" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="62">
+      <c r="A15" s="60">
         <v>4</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="80" t="s">
+      <c r="D15" s="72"/>
+      <c r="E15" s="47" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="15"/>
       <c r="M15" s="17"/>
       <c r="N15" s="15"/>
       <c r="U15" s="17"/>
-      <c r="V15" s="84"/>
-      <c r="W15" s="77"/>
-      <c r="X15" s="77"/>
-      <c r="Y15" s="77"/>
-      <c r="Z15" s="77"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="46"/>
+      <c r="Z15" s="46"/>
       <c r="AC15" s="17"/>
       <c r="AD15" s="15"/>
       <c r="AK15" s="17"/>
@@ -1852,11 +1858,11 @@
       <c r="CG15" s="17"/>
     </row>
     <row r="16" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="81" t="s">
+      <c r="A16" s="60"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="48" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="18"/>
@@ -1881,11 +1887,11 @@
       <c r="CG16" s="20"/>
     </row>
     <row r="17" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="82" t="s">
+      <c r="A17" s="60"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="49" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="18"/>
@@ -1910,11 +1916,11 @@
       <c r="CG17" s="20"/>
     </row>
     <row r="18" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="81" t="s">
+      <c r="A18" s="60"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="48" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="18"/>
@@ -1999,14 +2005,14 @@
       <c r="CG18" s="20"/>
     </row>
     <row r="19" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="62">
+      <c r="A19" s="60">
         <v>5</v>
       </c>
-      <c r="B19" s="46" t="s">
-        <v>26</v>
+      <c r="B19" s="57" t="s">
+        <v>25</v>
       </c>
       <c r="C19" s="68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="39" t="s">
@@ -2018,11 +2024,7 @@
       <c r="U19" s="11"/>
       <c r="V19" s="9"/>
       <c r="AC19" s="11"/>
-      <c r="AD19" s="84"/>
-      <c r="AE19" s="77"/>
-      <c r="AF19" s="77"/>
-      <c r="AG19" s="77"/>
-      <c r="AH19" s="77"/>
+      <c r="AD19" s="9"/>
       <c r="AK19" s="11"/>
       <c r="AL19" s="9"/>
       <c r="AS19" s="11"/>
@@ -2038,8 +2040,8 @@
       <c r="CG19" s="11"/>
     </row>
     <row r="20" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="47"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="69"/>
       <c r="D20" s="69"/>
       <c r="E20" s="40" t="s">
@@ -2057,8 +2059,8 @@
       <c r="CG20" s="13"/>
     </row>
     <row r="21" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="69"/>
       <c r="D21" s="69"/>
       <c r="E21" s="41" t="s">
@@ -2076,8 +2078,8 @@
       <c r="CG21" s="13"/>
     </row>
     <row r="22" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
-      <c r="B22" s="48"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="70"/>
       <c r="D22" s="70"/>
       <c r="E22" s="40" t="s">
@@ -2165,17 +2167,17 @@
       <c r="CG22" s="13"/>
     </row>
     <row r="23" spans="1:85" s="16" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62">
+      <c r="A23" s="60">
         <v>6</v>
       </c>
-      <c r="B23" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="80" t="s">
+      <c r="B23" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="71" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="72"/>
+      <c r="E23" s="47" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="15"/>
@@ -2200,11 +2202,11 @@
       <c r="CG23" s="17"/>
     </row>
     <row r="24" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="81" t="s">
+      <c r="A24" s="60"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="48" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="18"/>
@@ -2229,11 +2231,11 @@
       <c r="CG24" s="20"/>
     </row>
     <row r="25" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="82" t="s">
+      <c r="A25" s="60"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="49" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="18"/>
@@ -2258,11 +2260,11 @@
       <c r="CG25" s="20"/>
     </row>
     <row r="26" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="81" t="s">
+      <c r="A26" s="60"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="48" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="18"/>
@@ -2347,14 +2349,14 @@
       <c r="CG26" s="20"/>
     </row>
     <row r="27" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="62">
+      <c r="A27" s="60">
         <v>7</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="68" t="s">
         <v>28</v>
-      </c>
-      <c r="C27" s="68" t="s">
-        <v>29</v>
       </c>
       <c r="D27" s="68"/>
       <c r="E27" s="39" t="s">
@@ -2366,7 +2368,9 @@
       <c r="U27" s="11"/>
       <c r="V27" s="9"/>
       <c r="AC27" s="11"/>
-      <c r="AD27" s="9"/>
+      <c r="AD27" s="50"/>
+      <c r="AE27" s="46"/>
+      <c r="AF27" s="46"/>
       <c r="AK27" s="11"/>
       <c r="AL27" s="9"/>
       <c r="AS27" s="11"/>
@@ -2382,8 +2386,8 @@
       <c r="CG27" s="11"/>
     </row>
     <row r="28" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
-      <c r="B28" s="47"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="58"/>
       <c r="C28" s="69"/>
       <c r="D28" s="69"/>
       <c r="E28" s="40" t="s">
@@ -2401,8 +2405,8 @@
       <c r="CG28" s="13"/>
     </row>
     <row r="29" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
-      <c r="B29" s="47"/>
+      <c r="A29" s="60"/>
+      <c r="B29" s="58"/>
       <c r="C29" s="69"/>
       <c r="D29" s="69"/>
       <c r="E29" s="41" t="s">
@@ -2420,8 +2424,8 @@
       <c r="CG29" s="13"/>
     </row>
     <row r="30" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
-      <c r="B30" s="48"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="70"/>
       <c r="D30" s="70"/>
       <c r="E30" s="40" t="s">
@@ -2509,26 +2513,26 @@
       <c r="CG30" s="13"/>
     </row>
     <row r="31" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62" t="s">
+      <c r="A31" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="74"/>
-      <c r="E31" s="80" t="s">
+      <c r="C31" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="72"/>
+      <c r="E31" s="47" t="s">
         <v>16</v>
       </c>
       <c r="F31" s="15"/>
       <c r="M31" s="17"/>
-      <c r="N31" s="84"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="77"/>
-      <c r="Q31" s="77"/>
-      <c r="R31" s="77"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
       <c r="U31" s="17"/>
       <c r="V31" s="15"/>
       <c r="AC31" s="17"/>
@@ -2548,16 +2552,21 @@
       <c r="CG31" s="17"/>
     </row>
     <row r="32" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="81" t="s">
+      <c r="A32" s="60"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="48" t="s">
         <v>18</v>
       </c>
       <c r="F32" s="18"/>
       <c r="M32" s="20"/>
-      <c r="N32" s="18"/>
+      <c r="N32" s="52"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
       <c r="U32" s="20"/>
       <c r="V32" s="18"/>
       <c r="AC32" s="20"/>
@@ -2577,11 +2586,11 @@
       <c r="CG32" s="20"/>
     </row>
     <row r="33" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="82" t="s">
+      <c r="A33" s="60"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="73"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="49" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="18"/>
@@ -2606,11 +2615,11 @@
       <c r="CG33" s="20"/>
     </row>
     <row r="34" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="81" t="s">
+      <c r="A34" s="60"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="48" t="s">
         <v>19</v>
       </c>
       <c r="F34" s="18"/>
@@ -2695,14 +2704,14 @@
       <c r="CG34" s="20"/>
     </row>
     <row r="35" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="62">
+      <c r="A35" s="60">
         <v>9</v>
       </c>
-      <c r="B35" s="46" t="s">
-        <v>32</v>
+      <c r="B35" s="57" t="s">
+        <v>31</v>
       </c>
       <c r="C35" s="68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35" s="68"/>
       <c r="E35" s="39" t="s">
@@ -2716,12 +2725,15 @@
       <c r="AC35" s="11"/>
       <c r="AD35" s="9"/>
       <c r="AK35" s="11"/>
-      <c r="AL35" s="84"/>
-      <c r="AM35" s="77"/>
-      <c r="AN35" s="77"/>
-      <c r="AO35" s="77"/>
+      <c r="AL35" s="50"/>
+      <c r="AM35" s="46"/>
+      <c r="AN35" s="46"/>
+      <c r="AO35" s="46"/>
       <c r="AS35" s="11"/>
-      <c r="AT35" s="9"/>
+      <c r="AT35" s="50"/>
+      <c r="AU35" s="46"/>
+      <c r="AV35" s="46"/>
+      <c r="AW35" s="46"/>
       <c r="BA35" s="11"/>
       <c r="BB35" s="9"/>
       <c r="BI35" s="11"/>
@@ -2733,8 +2745,8 @@
       <c r="CG35" s="11"/>
     </row>
     <row r="36" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="58"/>
       <c r="C36" s="69"/>
       <c r="D36" s="69"/>
       <c r="E36" s="40" t="s">
@@ -2752,8 +2764,8 @@
       <c r="CG36" s="13"/>
     </row>
     <row r="37" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="62"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="69"/>
       <c r="D37" s="69"/>
       <c r="E37" s="41" t="s">
@@ -2768,6 +2780,10 @@
       <c r="AN37" s="42"/>
       <c r="AO37" s="42"/>
       <c r="AS37" s="13"/>
+      <c r="AT37" s="42"/>
+      <c r="AU37" s="42"/>
+      <c r="AV37" s="42"/>
+      <c r="AW37" s="42"/>
       <c r="BA37" s="13"/>
       <c r="BI37" s="13"/>
       <c r="BQ37" s="13"/>
@@ -2775,8 +2791,8 @@
       <c r="CG37" s="13"/>
     </row>
     <row r="38" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="62"/>
-      <c r="B38" s="48"/>
+      <c r="A38" s="60"/>
+      <c r="B38" s="59"/>
       <c r="C38" s="70"/>
       <c r="D38" s="70"/>
       <c r="E38" s="40" t="s">
@@ -2864,12 +2880,12 @@
       <c r="CG38" s="13"/>
     </row>
     <row r="39" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="62">
+      <c r="A39" s="60">
         <v>10</v>
       </c>
-      <c r="B39" s="71"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="49"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="65"/>
       <c r="E39" s="26" t="s">
         <v>5</v>
       </c>
@@ -2895,10 +2911,10 @@
       <c r="CG39" s="17"/>
     </row>
     <row r="40" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="62"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58"/>
+      <c r="A40" s="60"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="67"/>
       <c r="E40" s="27" t="s">
         <v>8</v>
       </c>
@@ -2924,10 +2940,10 @@
       <c r="CG40" s="20"/>
     </row>
     <row r="41" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="62"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58"/>
+      <c r="A41" s="60"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="67"/>
       <c r="E41" s="27" t="s">
         <v>9</v>
       </c>
@@ -2952,11 +2968,11 @@
       <c r="BZ41" s="18"/>
       <c r="CG41" s="20"/>
     </row>
-    <row r="42" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="62"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
+    <row r="42" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="60"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
       <c r="E42" s="43" t="s">
         <v>10</v>
       </c>
@@ -3042,12 +3058,12 @@
       <c r="CG42" s="20"/>
     </row>
     <row r="43" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="62">
+      <c r="A43" s="60">
         <v>11</v>
       </c>
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
       <c r="E43" s="39" t="s">
         <v>5</v>
       </c>
@@ -3072,11 +3088,11 @@
       <c r="BZ43" s="9"/>
       <c r="CG43" s="11"/>
     </row>
-    <row r="44" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="62"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
+    <row r="44" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="60"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
       <c r="E44" s="40" t="s">
         <v>7</v>
       </c>
@@ -3092,10 +3108,10 @@
       <c r="CG44" s="13"/>
     </row>
     <row r="45" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="62"/>
-      <c r="B45" s="60"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
+      <c r="A45" s="60"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
       <c r="E45" s="41" t="s">
         <v>9</v>
       </c>
@@ -3110,11 +3126,11 @@
       <c r="BY45" s="13"/>
       <c r="CG45" s="13"/>
     </row>
-    <row r="46" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A46" s="62"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
+    <row r="46" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="60"/>
+      <c r="B46" s="79"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
       <c r="E46" s="40" t="s">
         <v>10</v>
       </c>
@@ -3200,12 +3216,12 @@
       <c r="CG46" s="13"/>
     </row>
     <row r="47" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="62">
+      <c r="A47" s="60">
         <v>12</v>
       </c>
-      <c r="B47" s="71"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="49"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="65"/>
       <c r="E47" s="26" t="s">
         <v>5</v>
       </c>
@@ -3231,10 +3247,10 @@
       <c r="CG47" s="17"/>
     </row>
     <row r="48" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="62"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="58"/>
+      <c r="A48" s="60"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="67"/>
       <c r="E48" s="27" t="s">
         <v>7</v>
       </c>
@@ -3260,10 +3276,10 @@
       <c r="CG48" s="20"/>
     </row>
     <row r="49" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="62"/>
-      <c r="B49" s="50"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="58"/>
+      <c r="A49" s="60"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="67"/>
       <c r="E49" s="27" t="s">
         <v>9</v>
       </c>
@@ -3288,11 +3304,11 @@
       <c r="BZ49" s="18"/>
       <c r="CG49" s="20"/>
     </row>
-    <row r="50" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="62"/>
-      <c r="B50" s="51"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
+    <row r="50" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="60"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="67"/>
+      <c r="D50" s="67"/>
       <c r="E50" s="43" t="s">
         <v>10</v>
       </c>
@@ -3378,12 +3394,12 @@
       <c r="CG50" s="20"/>
     </row>
     <row r="51" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="62">
+      <c r="A51" s="60">
         <v>13</v>
       </c>
-      <c r="B51" s="59"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
+      <c r="B51" s="83"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
       <c r="E51" s="39" t="s">
         <v>5</v>
       </c>
@@ -3408,11 +3424,11 @@
       <c r="BZ51" s="9"/>
       <c r="CG51" s="11"/>
     </row>
-    <row r="52" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A52" s="62"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
+    <row r="52" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="60"/>
+      <c r="B52" s="78"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
       <c r="E52" s="40" t="s">
         <v>7</v>
       </c>
@@ -3428,10 +3444,10 @@
       <c r="CG52" s="13"/>
     </row>
     <row r="53" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="62"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
+      <c r="A53" s="60"/>
+      <c r="B53" s="78"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
       <c r="E53" s="41" t="s">
         <v>9</v>
       </c>
@@ -3446,11 +3462,11 @@
       <c r="BY53" s="13"/>
       <c r="CG53" s="13"/>
     </row>
-    <row r="54" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A54" s="62"/>
-      <c r="B54" s="61"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
+    <row r="54" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="60"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="59"/>
       <c r="E54" s="40" t="s">
         <v>10</v>
       </c>
@@ -3536,12 +3552,12 @@
       <c r="CG54" s="13"/>
     </row>
     <row r="55" spans="1:85" s="16" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="62">
+      <c r="A55" s="60">
         <v>14</v>
       </c>
-      <c r="B55" s="49"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="49"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="64"/>
+      <c r="D55" s="65"/>
       <c r="E55" s="26" t="s">
         <v>5</v>
       </c>
@@ -3567,10 +3583,10 @@
       <c r="CG55" s="17"/>
     </row>
     <row r="56" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="62"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="58"/>
+      <c r="A56" s="60"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="67"/>
       <c r="E56" s="27" t="s">
         <v>7</v>
       </c>
@@ -3596,10 +3612,10 @@
       <c r="CG56" s="20"/>
     </row>
     <row r="57" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="62"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="58"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="67"/>
       <c r="E57" s="27" t="s">
         <v>9</v>
       </c>
@@ -3624,11 +3640,11 @@
       <c r="BZ57" s="18"/>
       <c r="CG57" s="20"/>
     </row>
-    <row r="58" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="62"/>
-      <c r="B58" s="51"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
+    <row r="58" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="60"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="67"/>
+      <c r="D58" s="67"/>
       <c r="E58" s="43" t="s">
         <v>10</v>
       </c>
@@ -3714,12 +3730,12 @@
       <c r="CG58" s="20"/>
     </row>
     <row r="59" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="62">
+      <c r="A59" s="60">
         <v>15</v>
       </c>
-      <c r="B59" s="59"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="46"/>
+      <c r="B59" s="83"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
       <c r="E59" s="39" t="s">
         <v>5</v>
       </c>
@@ -3744,11 +3760,11 @@
       <c r="BZ59" s="9"/>
       <c r="CG59" s="11"/>
     </row>
-    <row r="60" spans="1:85" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A60" s="62"/>
-      <c r="B60" s="60"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
+    <row r="60" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="60"/>
+      <c r="B60" s="78"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="58"/>
       <c r="E60" s="40" t="s">
         <v>7</v>
       </c>
@@ -3764,10 +3780,10 @@
       <c r="CG60" s="13"/>
     </row>
     <row r="61" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="62"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
+      <c r="A61" s="60"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="58"/>
       <c r="E61" s="41" t="s">
         <v>9</v>
       </c>
@@ -3782,11 +3798,11 @@
       <c r="BY61" s="13"/>
       <c r="CG61" s="13"/>
     </row>
-    <row r="62" spans="1:85" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A62" s="62"/>
-      <c r="B62" s="61"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
+    <row r="62" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="60"/>
+      <c r="B62" s="79"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="59"/>
       <c r="E62" s="40" t="s">
         <v>10</v>
       </c>
@@ -3872,12 +3888,12 @@
       <c r="CG62" s="13"/>
     </row>
     <row r="63" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="62">
+      <c r="A63" s="60">
         <v>16</v>
       </c>
-      <c r="B63" s="49"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="49"/>
+      <c r="B63" s="65"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="65"/>
       <c r="E63" s="26" t="s">
         <v>5</v>
       </c>
@@ -3903,10 +3919,10 @@
       <c r="CG63" s="17"/>
     </row>
     <row r="64" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="62"/>
-      <c r="B64" s="50"/>
-      <c r="C64" s="57"/>
-      <c r="D64" s="58"/>
+      <c r="A64" s="60"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="67"/>
       <c r="E64" s="27" t="s">
         <v>7</v>
       </c>
@@ -3932,10 +3948,10 @@
       <c r="CG64" s="20"/>
     </row>
     <row r="65" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="62"/>
-      <c r="B65" s="50"/>
-      <c r="C65" s="57"/>
-      <c r="D65" s="58"/>
+      <c r="A65" s="60"/>
+      <c r="B65" s="62"/>
+      <c r="C65" s="66"/>
+      <c r="D65" s="67"/>
       <c r="E65" s="27" t="s">
         <v>9</v>
       </c>
@@ -3960,11 +3976,11 @@
       <c r="BZ65" s="18"/>
       <c r="CG65" s="20"/>
     </row>
-    <row r="66" spans="1:85" s="21" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="62"/>
-      <c r="B66" s="51"/>
-      <c r="C66" s="58"/>
-      <c r="D66" s="58"/>
+    <row r="66" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="60"/>
+      <c r="B66" s="63"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
       <c r="E66" s="43" t="s">
         <v>10</v>
       </c>
@@ -4050,12 +4066,12 @@
       <c r="CG66" s="20"/>
     </row>
     <row r="67" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="63"/>
-      <c r="B67" s="52" t="s">
+      <c r="A67" s="82"/>
+      <c r="B67" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="54"/>
-      <c r="D67" s="54"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="86"/>
       <c r="E67" s="30"/>
       <c r="F67" s="31"/>
       <c r="G67" s="32"/>
@@ -4141,10 +4157,10 @@
       <c r="CG67" s="37"/>
     </row>
     <row r="68" spans="1:85" s="14" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="63"/>
-      <c r="B68" s="53"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="55"/>
+      <c r="A68" s="82"/>
+      <c r="B68" s="85"/>
+      <c r="C68" s="87"/>
+      <c r="D68" s="87"/>
       <c r="E68" s="33"/>
       <c r="F68" s="34"/>
       <c r="G68" s="35"/>
@@ -4229,48 +4245,15 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="BJ1:BQ1"/>
-    <mergeCell ref="BR1:BY1"/>
-    <mergeCell ref="BZ1:CG1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AC1"/>
-    <mergeCell ref="AD1:AK1"/>
-    <mergeCell ref="AL1:AS1"/>
-    <mergeCell ref="AT1:BA1"/>
-    <mergeCell ref="C43:D46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:D50"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:D38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:D42"/>
-    <mergeCell ref="C23:D26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:D30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:D34"/>
-    <mergeCell ref="C11:D14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:D18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:D22"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="BB1:BI1"/>
-    <mergeCell ref="C7:D10"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:D6"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C51:D54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:D68"/>
+    <mergeCell ref="C55:D58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:D62"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:D66"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A63:A66"/>
@@ -4284,15 +4267,48 @@
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C51:D54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:D68"/>
-    <mergeCell ref="C55:D58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:D62"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:D66"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="BB1:BI1"/>
+    <mergeCell ref="C7:D10"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:D6"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C11:D14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:D18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:D22"/>
+    <mergeCell ref="C23:D26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:D30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:D34"/>
+    <mergeCell ref="C43:D46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:D50"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:D38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:D42"/>
+    <mergeCell ref="BJ1:BQ1"/>
+    <mergeCell ref="BR1:BY1"/>
+    <mergeCell ref="BZ1:CG1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="AD1:AK1"/>
+    <mergeCell ref="AL1:AS1"/>
+    <mergeCell ref="AT1:BA1"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Dokumentation, Gantt, Scrum nachgeführt
</commit_message>
<xml_diff>
--- a/Restaurants_Vallah_SJ/Documentation/210_Gantt-Diagramm.110_Sebastian_Joel.xlsx
+++ b/Restaurants_Vallah_SJ/Documentation/210_Gantt-Diagramm.110_Sebastian_Joel.xlsx
@@ -103,9 +103,6 @@
     <t>US 07 "Als Benutzer möchte ich ein Restaurant auswählen können und dafür alle Informationen angezeigt bekommen."</t>
   </si>
   <si>
-    <t>3h /</t>
-  </si>
-  <si>
     <t>"</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>8h / 10h</t>
+  </si>
+  <si>
+    <t>3h / 7h</t>
   </si>
 </sst>
 </file>
@@ -467,110 +467,110 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW26" sqref="AW26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +930,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="24"/>
@@ -941,109 +941,109 @@
       <c r="E1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="56">
+      <c r="F1" s="73">
         <v>43129</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="56">
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="73">
         <v>43136</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="56">
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="73">
         <v>43137</v>
       </c>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="56">
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="74"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="73">
         <v>43138</v>
       </c>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="56">
+      <c r="AE1" s="74"/>
+      <c r="AF1" s="74"/>
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="74"/>
+      <c r="AI1" s="74"/>
+      <c r="AJ1" s="74"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="73">
         <v>43139</v>
       </c>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-      <c r="AQ1" s="54"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="55"/>
-      <c r="AT1" s="56">
+      <c r="AM1" s="74"/>
+      <c r="AN1" s="74"/>
+      <c r="AO1" s="74"/>
+      <c r="AP1" s="74"/>
+      <c r="AQ1" s="74"/>
+      <c r="AR1" s="74"/>
+      <c r="AS1" s="75"/>
+      <c r="AT1" s="73">
         <v>43150</v>
       </c>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
-      <c r="AW1" s="54"/>
-      <c r="AX1" s="54"/>
-      <c r="AY1" s="54"/>
-      <c r="AZ1" s="54"/>
-      <c r="BA1" s="55"/>
-      <c r="BB1" s="56">
+      <c r="AU1" s="74"/>
+      <c r="AV1" s="74"/>
+      <c r="AW1" s="74"/>
+      <c r="AX1" s="74"/>
+      <c r="AY1" s="74"/>
+      <c r="AZ1" s="74"/>
+      <c r="BA1" s="75"/>
+      <c r="BB1" s="73">
         <v>43151</v>
       </c>
-      <c r="BC1" s="54"/>
-      <c r="BD1" s="54"/>
-      <c r="BE1" s="54"/>
-      <c r="BF1" s="54"/>
-      <c r="BG1" s="54"/>
-      <c r="BH1" s="54"/>
-      <c r="BI1" s="55"/>
-      <c r="BJ1" s="56">
+      <c r="BC1" s="74"/>
+      <c r="BD1" s="74"/>
+      <c r="BE1" s="74"/>
+      <c r="BF1" s="74"/>
+      <c r="BG1" s="74"/>
+      <c r="BH1" s="74"/>
+      <c r="BI1" s="75"/>
+      <c r="BJ1" s="73">
         <v>43152</v>
       </c>
-      <c r="BK1" s="54"/>
-      <c r="BL1" s="54"/>
-      <c r="BM1" s="54"/>
-      <c r="BN1" s="54"/>
-      <c r="BO1" s="54"/>
-      <c r="BP1" s="54"/>
-      <c r="BQ1" s="55"/>
-      <c r="BR1" s="53" t="s">
+      <c r="BK1" s="74"/>
+      <c r="BL1" s="74"/>
+      <c r="BM1" s="74"/>
+      <c r="BN1" s="74"/>
+      <c r="BO1" s="74"/>
+      <c r="BP1" s="74"/>
+      <c r="BQ1" s="75"/>
+      <c r="BR1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="BS1" s="54"/>
-      <c r="BT1" s="54"/>
-      <c r="BU1" s="54"/>
-      <c r="BV1" s="54"/>
-      <c r="BW1" s="54"/>
-      <c r="BX1" s="54"/>
-      <c r="BY1" s="55"/>
-      <c r="BZ1" s="53" t="s">
+      <c r="BS1" s="74"/>
+      <c r="BT1" s="74"/>
+      <c r="BU1" s="74"/>
+      <c r="BV1" s="74"/>
+      <c r="BW1" s="74"/>
+      <c r="BX1" s="74"/>
+      <c r="BY1" s="75"/>
+      <c r="BZ1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="CA1" s="54"/>
-      <c r="CB1" s="54"/>
-      <c r="CC1" s="54"/>
-      <c r="CD1" s="54"/>
-      <c r="CE1" s="54"/>
-      <c r="CF1" s="54"/>
-      <c r="CG1" s="55"/>
+      <c r="CA1" s="74"/>
+      <c r="CB1" s="74"/>
+      <c r="CC1" s="74"/>
+      <c r="CD1" s="74"/>
+      <c r="CE1" s="74"/>
+      <c r="CF1" s="74"/>
+      <c r="CG1" s="75"/>
     </row>
     <row r="2" spans="1:85" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="76"/>
+      <c r="A2" s="72"/>
       <c r="B2" s="22" t="s">
         <v>13</v>
       </c>
@@ -1296,23 +1296,23 @@
       </c>
     </row>
     <row r="3" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60">
+      <c r="A3" s="69">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="68" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="68"/>
+      <c r="C3" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="79"/>
       <c r="E3" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="80"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="83"/>
       <c r="M3" s="11"/>
       <c r="N3" s="9"/>
       <c r="U3" s="11"/>
@@ -1334,10 +1334,10 @@
       <c r="CG3" s="11"/>
     </row>
     <row r="4" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
       <c r="E4" s="40" t="s">
         <v>18</v>
       </c>
@@ -1353,10 +1353,10 @@
       <c r="CG4" s="13"/>
     </row>
     <row r="5" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
       <c r="E5" s="41" t="s">
         <v>17</v>
       </c>
@@ -1377,10 +1377,10 @@
       <c r="CG5" s="13"/>
     </row>
     <row r="6" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
       <c r="E6" s="40" t="s">
         <v>19</v>
       </c>
@@ -1466,16 +1466,16 @@
       <c r="CG6" s="13"/>
     </row>
     <row r="7" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="60">
+      <c r="A7" s="69">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="72"/>
+      <c r="D7" s="76"/>
       <c r="E7" s="47" t="s">
         <v>16</v>
       </c>
@@ -1503,10 +1503,10 @@
       <c r="CG7" s="17"/>
     </row>
     <row r="8" spans="1:85" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
       <c r="E8" s="48" t="s">
         <v>18</v>
       </c>
@@ -1531,10 +1531,10 @@
       <c r="CG8" s="20"/>
     </row>
     <row r="9" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
       <c r="E9" s="49" t="s">
         <v>17</v>
       </c>
@@ -1560,10 +1560,10 @@
       <c r="CG9" s="20"/>
     </row>
     <row r="10" spans="1:85" s="21" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
       <c r="E10" s="48" t="s">
         <v>19</v>
       </c>
@@ -1649,16 +1649,16 @@
       <c r="CG10" s="20"/>
     </row>
     <row r="11" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="60">
+      <c r="A11" s="69">
         <v>3</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="68"/>
+      <c r="C11" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="79"/>
       <c r="E11" s="39" t="s">
         <v>16</v>
       </c>
@@ -1684,10 +1684,10 @@
       <c r="CG11" s="11"/>
     </row>
     <row r="12" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
       <c r="E12" s="40" t="s">
         <v>18</v>
       </c>
@@ -1703,10 +1703,10 @@
       <c r="CG12" s="13"/>
     </row>
     <row r="13" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
       <c r="E13" s="41" t="s">
         <v>17</v>
       </c>
@@ -1730,10 +1730,10 @@
       <c r="CG13" s="13"/>
     </row>
     <row r="14" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
       <c r="E14" s="40" t="s">
         <v>19</v>
       </c>
@@ -1819,16 +1819,16 @@
       <c r="CG14" s="13"/>
     </row>
     <row r="15" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60">
+      <c r="A15" s="69">
         <v>4</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="72"/>
+      <c r="D15" s="76"/>
       <c r="E15" s="47" t="s">
         <v>16</v>
       </c>
@@ -1858,10 +1858,10 @@
       <c r="CG15" s="17"/>
     </row>
     <row r="16" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="74"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="77"/>
       <c r="E16" s="48" t="s">
         <v>18</v>
       </c>
@@ -1887,10 +1887,10 @@
       <c r="CG16" s="20"/>
     </row>
     <row r="17" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="74"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="77"/>
       <c r="E17" s="49" t="s">
         <v>17</v>
       </c>
@@ -1916,10 +1916,10 @@
       <c r="CG17" s="20"/>
     </row>
     <row r="18" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="77"/>
       <c r="E18" s="48" t="s">
         <v>19</v>
       </c>
@@ -2005,16 +2005,16 @@
       <c r="CG18" s="20"/>
     </row>
     <row r="19" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="60">
+      <c r="A19" s="69">
         <v>5</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="68" t="s">
+      <c r="C19" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="68"/>
+      <c r="D19" s="79"/>
       <c r="E19" s="39" t="s">
         <v>16</v>
       </c>
@@ -2040,10 +2040,10 @@
       <c r="CG19" s="11"/>
     </row>
     <row r="20" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="60"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
       <c r="E20" s="40" t="s">
         <v>18</v>
       </c>
@@ -2059,10 +2059,10 @@
       <c r="CG20" s="13"/>
     </row>
     <row r="21" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="60"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
       <c r="E21" s="41" t="s">
         <v>17</v>
       </c>
@@ -2078,10 +2078,10 @@
       <c r="CG21" s="13"/>
     </row>
     <row r="22" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="60"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
       <c r="E22" s="40" t="s">
         <v>19</v>
       </c>
@@ -2167,16 +2167,16 @@
       <c r="CG22" s="13"/>
     </row>
     <row r="23" spans="1:85" s="16" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="60">
+      <c r="A23" s="69">
         <v>6</v>
       </c>
-      <c r="B23" s="65" t="s">
+      <c r="B23" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="72"/>
+      <c r="D23" s="76"/>
       <c r="E23" s="47" t="s">
         <v>16</v>
       </c>
@@ -2202,10 +2202,10 @@
       <c r="CG23" s="17"/>
     </row>
     <row r="24" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="60"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="74"/>
+      <c r="A24" s="69"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="77"/>
       <c r="E24" s="48" t="s">
         <v>18</v>
       </c>
@@ -2231,10 +2231,10 @@
       <c r="CG24" s="20"/>
     </row>
     <row r="25" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="60"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="74"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="77"/>
       <c r="E25" s="49" t="s">
         <v>17</v>
       </c>
@@ -2260,10 +2260,10 @@
       <c r="CG25" s="20"/>
     </row>
     <row r="26" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="60"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
       <c r="E26" s="48" t="s">
         <v>19</v>
       </c>
@@ -2349,16 +2349,16 @@
       <c r="CG26" s="20"/>
     </row>
     <row r="27" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60">
+      <c r="A27" s="69">
         <v>7</v>
       </c>
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="68"/>
+      <c r="C27" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="79"/>
       <c r="E27" s="39" t="s">
         <v>16</v>
       </c>
@@ -2386,16 +2386,23 @@
       <c r="CG27" s="11"/>
     </row>
     <row r="28" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="60"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80"/>
       <c r="E28" s="40" t="s">
         <v>18</v>
       </c>
       <c r="M28" s="13"/>
       <c r="U28" s="13"/>
       <c r="AC28" s="13"/>
+      <c r="AD28" s="23"/>
+      <c r="AE28" s="23"/>
+      <c r="AF28" s="23"/>
+      <c r="AG28" s="23"/>
+      <c r="AH28" s="23"/>
+      <c r="AI28" s="23"/>
+      <c r="AJ28" s="23"/>
       <c r="AK28" s="13"/>
       <c r="AS28" s="13"/>
       <c r="BA28" s="13"/>
@@ -2405,10 +2412,10 @@
       <c r="CG28" s="13"/>
     </row>
     <row r="29" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="60"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
       <c r="E29" s="41" t="s">
         <v>17</v>
       </c>
@@ -2424,10 +2431,10 @@
       <c r="CG29" s="13"/>
     </row>
     <row r="30" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="60"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
       <c r="E30" s="40" t="s">
         <v>19</v>
       </c>
@@ -2513,16 +2520,16 @@
       <c r="CG30" s="13"/>
     </row>
     <row r="31" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="72"/>
+      <c r="C31" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="76"/>
       <c r="E31" s="47" t="s">
         <v>16</v>
       </c>
@@ -2552,10 +2559,10 @@
       <c r="CG31" s="17"/>
     </row>
     <row r="32" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="60"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="74"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="85"/>
+      <c r="D32" s="77"/>
       <c r="E32" s="48" t="s">
         <v>18</v>
       </c>
@@ -2586,10 +2593,10 @@
       <c r="CG32" s="20"/>
     </row>
     <row r="33" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="60"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="73"/>
-      <c r="D33" s="74"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="77"/>
       <c r="E33" s="49" t="s">
         <v>17</v>
       </c>
@@ -2615,10 +2622,10 @@
       <c r="CG33" s="20"/>
     </row>
     <row r="34" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="60"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
       <c r="E34" s="48" t="s">
         <v>19</v>
       </c>
@@ -2704,16 +2711,16 @@
       <c r="CG34" s="20"/>
     </row>
     <row r="35" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="60">
+      <c r="A35" s="69">
         <v>9</v>
       </c>
-      <c r="B35" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="68"/>
+      <c r="B35" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="79"/>
       <c r="E35" s="39" t="s">
         <v>16</v>
       </c>
@@ -2745,10 +2752,10 @@
       <c r="CG35" s="11"/>
     </row>
     <row r="36" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="60"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
+      <c r="A36" s="69"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
       <c r="E36" s="40" t="s">
         <v>18</v>
       </c>
@@ -2756,7 +2763,9 @@
       <c r="U36" s="13"/>
       <c r="AC36" s="13"/>
       <c r="AK36" s="13"/>
+      <c r="AL36" s="23"/>
       <c r="AS36" s="13"/>
+      <c r="AT36" s="23"/>
       <c r="BA36" s="13"/>
       <c r="BI36" s="13"/>
       <c r="BQ36" s="13"/>
@@ -2764,10 +2773,10 @@
       <c r="CG36" s="13"/>
     </row>
     <row r="37" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="60"/>
-      <c r="B37" s="58"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
       <c r="E37" s="41" t="s">
         <v>17</v>
       </c>
@@ -2791,10 +2800,10 @@
       <c r="CG37" s="13"/>
     </row>
     <row r="38" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="60"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="81"/>
       <c r="E38" s="40" t="s">
         <v>19</v>
       </c>
@@ -2830,18 +2839,18 @@
       <c r="AI38" s="12"/>
       <c r="AJ38" s="12"/>
       <c r="AK38" s="13"/>
-      <c r="AL38" s="12"/>
-      <c r="AM38" s="12"/>
-      <c r="AN38" s="12"/>
-      <c r="AO38" s="12"/>
+      <c r="AL38" s="23"/>
+      <c r="AM38" s="23"/>
+      <c r="AN38" s="23"/>
+      <c r="AO38" s="23"/>
       <c r="AP38" s="12"/>
       <c r="AQ38" s="12"/>
       <c r="AR38" s="12"/>
       <c r="AS38" s="13"/>
-      <c r="AT38" s="12"/>
-      <c r="AU38" s="12"/>
-      <c r="AV38" s="12"/>
-      <c r="AW38" s="12"/>
+      <c r="AT38" s="23"/>
+      <c r="AU38" s="23"/>
+      <c r="AV38" s="23"/>
+      <c r="AW38" s="23"/>
       <c r="AX38" s="12"/>
       <c r="AY38" s="12"/>
       <c r="AZ38" s="12"/>
@@ -2880,12 +2889,12 @@
       <c r="CG38" s="13"/>
     </row>
     <row r="39" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="60">
+      <c r="A39" s="69">
         <v>10</v>
       </c>
-      <c r="B39" s="61"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="65"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="56"/>
       <c r="E39" s="26" t="s">
         <v>5</v>
       </c>
@@ -2911,10 +2920,10 @@
       <c r="CG39" s="17"/>
     </row>
     <row r="40" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="60"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="67"/>
+      <c r="A40" s="69"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="27" t="s">
         <v>8</v>
       </c>
@@ -2940,10 +2949,10 @@
       <c r="CG40" s="20"/>
     </row>
     <row r="41" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="60"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="66"/>
-      <c r="D41" s="67"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="65"/>
       <c r="E41" s="27" t="s">
         <v>9</v>
       </c>
@@ -2969,10 +2978,10 @@
       <c r="CG41" s="20"/>
     </row>
     <row r="42" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="60"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="43" t="s">
         <v>10</v>
       </c>
@@ -3058,12 +3067,12 @@
       <c r="CG42" s="20"/>
     </row>
     <row r="43" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="60">
+      <c r="A43" s="69">
         <v>11</v>
       </c>
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
       <c r="E43" s="39" t="s">
         <v>5</v>
       </c>
@@ -3089,10 +3098,10 @@
       <c r="CG43" s="11"/>
     </row>
     <row r="44" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="60"/>
-      <c r="B44" s="78"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
+      <c r="A44" s="69"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
       <c r="E44" s="40" t="s">
         <v>7</v>
       </c>
@@ -3108,10 +3117,10 @@
       <c r="CG44" s="13"/>
     </row>
     <row r="45" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="60"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
+      <c r="A45" s="69"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
       <c r="E45" s="41" t="s">
         <v>9</v>
       </c>
@@ -3127,10 +3136,10 @@
       <c r="CG45" s="13"/>
     </row>
     <row r="46" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="60"/>
-      <c r="B46" s="79"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
+      <c r="A46" s="69"/>
+      <c r="B46" s="68"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
       <c r="E46" s="40" t="s">
         <v>10</v>
       </c>
@@ -3216,12 +3225,12 @@
       <c r="CG46" s="13"/>
     </row>
     <row r="47" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="60">
+      <c r="A47" s="69">
         <v>12</v>
       </c>
-      <c r="B47" s="61"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="65"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="56"/>
       <c r="E47" s="26" t="s">
         <v>5</v>
       </c>
@@ -3247,10 +3256,10 @@
       <c r="CG47" s="17"/>
     </row>
     <row r="48" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="60"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="67"/>
+      <c r="A48" s="69"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="65"/>
       <c r="E48" s="27" t="s">
         <v>7</v>
       </c>
@@ -3276,10 +3285,10 @@
       <c r="CG48" s="20"/>
     </row>
     <row r="49" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="60"/>
-      <c r="B49" s="62"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="67"/>
+      <c r="A49" s="69"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="65"/>
       <c r="E49" s="27" t="s">
         <v>9</v>
       </c>
@@ -3305,10 +3314,10 @@
       <c r="CG49" s="20"/>
     </row>
     <row r="50" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="60"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="65"/>
       <c r="E50" s="43" t="s">
         <v>10</v>
       </c>
@@ -3394,12 +3403,12 @@
       <c r="CG50" s="20"/>
     </row>
     <row r="51" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="60">
+      <c r="A51" s="69">
         <v>13</v>
       </c>
-      <c r="B51" s="83"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
       <c r="E51" s="39" t="s">
         <v>5</v>
       </c>
@@ -3425,10 +3434,10 @@
       <c r="CG51" s="11"/>
     </row>
     <row r="52" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="60"/>
-      <c r="B52" s="78"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
+      <c r="A52" s="69"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
       <c r="E52" s="40" t="s">
         <v>7</v>
       </c>
@@ -3444,10 +3453,10 @@
       <c r="CG52" s="13"/>
     </row>
     <row r="53" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="60"/>
-      <c r="B53" s="78"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
+      <c r="A53" s="69"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="54"/>
       <c r="E53" s="41" t="s">
         <v>9</v>
       </c>
@@ -3463,10 +3472,10 @@
       <c r="CG53" s="13"/>
     </row>
     <row r="54" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="60"/>
-      <c r="B54" s="79"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="59"/>
+      <c r="A54" s="69"/>
+      <c r="B54" s="68"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
       <c r="E54" s="40" t="s">
         <v>10</v>
       </c>
@@ -3552,12 +3561,12 @@
       <c r="CG54" s="13"/>
     </row>
     <row r="55" spans="1:85" s="16" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="60">
+      <c r="A55" s="69">
         <v>14</v>
       </c>
-      <c r="B55" s="65"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="65"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="56"/>
       <c r="E55" s="26" t="s">
         <v>5</v>
       </c>
@@ -3583,10 +3592,10 @@
       <c r="CG55" s="17"/>
     </row>
     <row r="56" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="60"/>
-      <c r="B56" s="62"/>
-      <c r="C56" s="66"/>
-      <c r="D56" s="67"/>
+      <c r="A56" s="69"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="65"/>
       <c r="E56" s="27" t="s">
         <v>7</v>
       </c>
@@ -3612,10 +3621,10 @@
       <c r="CG56" s="20"/>
     </row>
     <row r="57" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="60"/>
-      <c r="B57" s="62"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="67"/>
+      <c r="A57" s="69"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="65"/>
       <c r="E57" s="27" t="s">
         <v>9</v>
       </c>
@@ -3641,10 +3650,10 @@
       <c r="CG57" s="20"/>
     </row>
     <row r="58" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="60"/>
-      <c r="B58" s="63"/>
-      <c r="C58" s="67"/>
-      <c r="D58" s="67"/>
+      <c r="A58" s="69"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="65"/>
       <c r="E58" s="43" t="s">
         <v>10</v>
       </c>
@@ -3730,12 +3739,12 @@
       <c r="CG58" s="20"/>
     </row>
     <row r="59" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="60">
+      <c r="A59" s="69">
         <v>15</v>
       </c>
-      <c r="B59" s="83"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="57"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
       <c r="E59" s="39" t="s">
         <v>5</v>
       </c>
@@ -3761,10 +3770,10 @@
       <c r="CG59" s="11"/>
     </row>
     <row r="60" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="60"/>
-      <c r="B60" s="78"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
+      <c r="A60" s="69"/>
+      <c r="B60" s="67"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
       <c r="E60" s="40" t="s">
         <v>7</v>
       </c>
@@ -3780,10 +3789,10 @@
       <c r="CG60" s="13"/>
     </row>
     <row r="61" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="60"/>
-      <c r="B61" s="78"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
+      <c r="A61" s="69"/>
+      <c r="B61" s="67"/>
+      <c r="C61" s="54"/>
+      <c r="D61" s="54"/>
       <c r="E61" s="41" t="s">
         <v>9</v>
       </c>
@@ -3799,10 +3808,10 @@
       <c r="CG61" s="13"/>
     </row>
     <row r="62" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="60"/>
-      <c r="B62" s="79"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="59"/>
+      <c r="A62" s="69"/>
+      <c r="B62" s="68"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
       <c r="E62" s="40" t="s">
         <v>10</v>
       </c>
@@ -3888,12 +3897,12 @@
       <c r="CG62" s="13"/>
     </row>
     <row r="63" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="60">
+      <c r="A63" s="69">
         <v>16</v>
       </c>
-      <c r="B63" s="65"/>
-      <c r="C63" s="64"/>
-      <c r="D63" s="65"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="56"/>
       <c r="E63" s="26" t="s">
         <v>5</v>
       </c>
@@ -3919,10 +3928,10 @@
       <c r="CG63" s="17"/>
     </row>
     <row r="64" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="60"/>
-      <c r="B64" s="62"/>
-      <c r="C64" s="66"/>
-      <c r="D64" s="67"/>
+      <c r="A64" s="69"/>
+      <c r="B64" s="57"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="65"/>
       <c r="E64" s="27" t="s">
         <v>7</v>
       </c>
@@ -3948,10 +3957,10 @@
       <c r="CG64" s="20"/>
     </row>
     <row r="65" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="60"/>
-      <c r="B65" s="62"/>
-      <c r="C65" s="66"/>
-      <c r="D65" s="67"/>
+      <c r="A65" s="69"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="65"/>
       <c r="E65" s="27" t="s">
         <v>9</v>
       </c>
@@ -3977,10 +3986,10 @@
       <c r="CG65" s="20"/>
     </row>
     <row r="66" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="60"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="67"/>
-      <c r="D66" s="67"/>
+      <c r="A66" s="69"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="65"/>
+      <c r="D66" s="65"/>
       <c r="E66" s="43" t="s">
         <v>10</v>
       </c>
@@ -4066,12 +4075,12 @@
       <c r="CG66" s="20"/>
     </row>
     <row r="67" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="82"/>
-      <c r="B67" s="84" t="s">
+      <c r="A67" s="70"/>
+      <c r="B67" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="86"/>
-      <c r="D67" s="86"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="61"/>
       <c r="E67" s="30"/>
       <c r="F67" s="31"/>
       <c r="G67" s="32"/>
@@ -4157,10 +4166,10 @@
       <c r="CG67" s="37"/>
     </row>
     <row r="68" spans="1:85" s="14" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="82"/>
-      <c r="B68" s="85"/>
-      <c r="C68" s="87"/>
-      <c r="D68" s="87"/>
+      <c r="A68" s="70"/>
+      <c r="B68" s="60"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="62"/>
       <c r="E68" s="33"/>
       <c r="F68" s="34"/>
       <c r="G68" s="35"/>
@@ -4245,15 +4254,48 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="C51:D54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:D68"/>
-    <mergeCell ref="C55:D58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:D62"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:D66"/>
+    <mergeCell ref="BJ1:BQ1"/>
+    <mergeCell ref="BR1:BY1"/>
+    <mergeCell ref="BZ1:CG1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="AD1:AK1"/>
+    <mergeCell ref="AL1:AS1"/>
+    <mergeCell ref="AT1:BA1"/>
+    <mergeCell ref="C43:D46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:D50"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:D38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:D42"/>
+    <mergeCell ref="C23:D26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:D30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:D34"/>
+    <mergeCell ref="C11:D14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:D18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:D22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="BB1:BI1"/>
+    <mergeCell ref="C7:D10"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:D6"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A63:A66"/>
@@ -4267,48 +4309,15 @@
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="BB1:BI1"/>
-    <mergeCell ref="C7:D10"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:D6"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C11:D14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:D18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:D22"/>
-    <mergeCell ref="C23:D26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:D30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:D34"/>
-    <mergeCell ref="C43:D46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:D50"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:D38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:D42"/>
-    <mergeCell ref="BJ1:BQ1"/>
-    <mergeCell ref="BR1:BY1"/>
-    <mergeCell ref="BZ1:CG1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AC1"/>
-    <mergeCell ref="AD1:AK1"/>
-    <mergeCell ref="AL1:AS1"/>
-    <mergeCell ref="AT1:BA1"/>
+    <mergeCell ref="C51:D54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:D68"/>
+    <mergeCell ref="C55:D58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:D62"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:D66"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>